<commit_message>
Clean up 0s and 1s for generated code for recurrence chained fullness 20220821
</commit_message>
<xml_diff>
--- a/LoopGen/recurrence-chained-fullness-20220821/cores.xlsx
+++ b/LoopGen/recurrence-chained-fullness-20220821/cores.xlsx
@@ -457,9 +457,9 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*B)[i] = (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*A)[i] = (*A)[i - 1];
   }
 </t>
         </is>
@@ -477,9 +477,9 @@
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 1];
+    (*A)[i] = (*A)[i - 1];
   }
 </t>
         </is>
@@ -497,9 +497,9 @@
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
+    (*B)[i] = (*B)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*A)[i - 1];
   }
 </t>
         </is>
@@ -517,9 +517,9 @@
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1];
   }
 </t>
         </is>
@@ -537,9 +537,9 @@
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (*B)[i - 1];
   }
 </t>
         </is>
@@ -557,9 +557,9 @@
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -577,9 +577,9 @@
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -597,9 +597,9 @@
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = (((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -617,9 +617,9 @@
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -637,9 +637,9 @@
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 1];
   }
 </t>
         </is>
@@ -657,9 +657,9 @@
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -677,9 +677,9 @@
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = (((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -697,9 +697,9 @@
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -717,9 +717,9 @@
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -737,9 +737,9 @@
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -757,9 +757,9 @@
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
+    (*B)[i] = (((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -777,9 +777,9 @@
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*C)[i] = (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2];
+    (*B)[i] = (*B)[i - 2];
   }
 </t>
         </is>
@@ -797,9 +797,9 @@
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*B)[i] = (*B)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*A)[i - 1];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -817,9 +817,9 @@
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*B)[i] = (*B)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 1];
+    (*A)[i] = (*A)[i - 2];
   }
 </t>
         </is>
@@ -837,9 +837,9 @@
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 2] + (*A)[i - 2]) + (*A)[i - 2];
   }
 </t>
         </is>
@@ -857,9 +857,9 @@
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
+    (*A)[i] = (*A)[i - 2];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -877,9 +877,9 @@
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 0 * (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 2];
   }
 </t>
         </is>
@@ -897,9 +897,9 @@
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 2];
+    (*B)[i] = (((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -917,9 +917,9 @@
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2];
+    (*B)[i] = (((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*A)[i - 2];
   }
 </t>
         </is>
@@ -937,9 +937,9 @@
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 2];
+    (*B)[i] = (((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -957,9 +957,9 @@
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 2];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -977,9 +977,9 @@
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -997,9 +997,9 @@
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*B)[i] = ((((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = ((((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -1017,9 +1017,9 @@
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*A)[i - 2]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1037,9 +1037,9 @@
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -1057,9 +1057,9 @@
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2];
+    (*A)[i] = (((((*A)[i - 2] + (*A)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = ((((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -1077,9 +1077,9 @@
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
+    (*B)[i] = (((((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*A)[i] = (((((*A)[i - 2] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -1097,9 +1097,9 @@
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (*A)[i - 3];
   }
 </t>
         </is>
@@ -1117,9 +1117,9 @@
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2];
+    (*B)[i] = (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3];
   }
 </t>
         </is>
@@ -1137,9 +1137,9 @@
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
+    (*A)[i] = (*A)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -1157,9 +1157,9 @@
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 2]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1177,9 +1177,9 @@
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*A)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1197,9 +1197,9 @@
       <c r="C39" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 3]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 2];
+    (*A)[i] = (*A)[i - 3] + (*A)[i - 1];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 2]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -1217,9 +1217,9 @@
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 3]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*A)[i - 2];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1237,9 +1237,9 @@
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 3]) + 0 * (*A)[i - 3]) + 1 * (*A)[i - 3];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 2];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 3];
+    (*A)[i] = (((*A)[i - 3] + (*A)[i - 1]) + (*A)[i - 3]) + (*A)[i - 3];
   }
 </t>
         </is>
@@ -1257,9 +1257,9 @@
       <c r="C42" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 3]) + 1 * (*A)[i - 2]) + 0 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 3] + (*A)[i - 1]) + (*A)[i - 2];
+    (*B)[i] = (((((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -1277,9 +1277,9 @@
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 2]) + 1 * (*A)[i - 3]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 3] + (*A)[i - 3]) + (*A)[i - 2]) + (*A)[i - 1];
+    (*C)[i] = ((((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1297,9 +1297,9 @@
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 3]) + 0 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 3]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 3]) + 1 * (*A)[i - 2];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 3];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 3]) + (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 3] + (*A)[i - 1]) + (*A)[i - 3]) + (*A)[i - 2]) + (*A)[i - 3]) + (*A)[i - 2];
   }
 </t>
         </is>
@@ -1317,9 +1317,9 @@
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 3] + 0 * (*A)[i - 3]) + 1 * (*A)[i - 3]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 3];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 3]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 3]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 3] + (*A)[i - 3]) + (*A)[i - 1]) + (*A)[i - 2]) + (*A)[i - 3];
   }
 </t>
         </is>
@@ -1337,9 +1337,9 @@
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 3];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 3]) + (*C)[i - 3]) + (*C)[i - 3]) + (*C)[i - 1];
+    (*B)[i] = (((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 3]) + (*B)[i - 2];
+    (*A)[i] = ((((*A)[i - 3] + (*A)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -1357,9 +1357,9 @@
       <c r="C47" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 2]) + (*B)[i - 3]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*A)[i] = (((((*A)[i - 3] + (*A)[i - 1]) + (*A)[i - 2]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 2];
+    (*C)[i] = ((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -1377,9 +1377,9 @@
       <c r="C48" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 3];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 3]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 3] + (*A)[i - 2]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 3];
+    (*B)[i] = (((((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 3]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1397,9 +1397,9 @@
       <c r="C49" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 3]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 3];
+    (*A)[i] = (((((*A)[i - 3] + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 3]) + (*A)[i - 2]) + (*A)[i - 3];
+    (*B)[i] = (((((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 3]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1417,9 +1417,9 @@
       <c r="C50" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*B)[i] = (*B)[i - 1];
   }
 </t>
         </is>
@@ -1437,9 +1437,9 @@
       <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*B)[i] = (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1457,9 +1457,9 @@
       <c r="C52" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1477,9 +1477,9 @@
       <c r="C53" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = (*C)[i - 1];
   }
 </t>
         </is>
@@ -1497,9 +1497,9 @@
       <c r="C54" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1517,9 +1517,9 @@
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 1];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -1537,9 +1537,9 @@
       <c r="C56" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
+    (*C)[i] = (((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -1557,9 +1557,9 @@
       <c r="C57" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1577,9 +1577,9 @@
       <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -1597,9 +1597,9 @@
       <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = (((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1617,9 +1617,9 @@
       <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1637,9 +1637,9 @@
       <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*B)[i] = (((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -1657,9 +1657,9 @@
       <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1677,9 +1677,9 @@
       <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1697,9 +1697,9 @@
       <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*B)[i] = (((((*B)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1717,9 +1717,9 @@
       <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
+    (*C)[i] = (*C)[i - 2];
+    (*B)[i] = (*B)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
   }
 </t>
         </is>
@@ -1737,9 +1737,9 @@
       <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
   }
 </t>
         </is>
@@ -1757,9 +1757,9 @@
       <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -1777,9 +1777,9 @@
       <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1];
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 1];
+    (*B)[i] = (*B)[i - 2];
   }
 </t>
         </is>
@@ -1797,9 +1797,9 @@
       <c r="C69" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = (*C)[i - 2];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1817,9 +1817,9 @@
       <c r="C70" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*B)[i - 1];
   }
 </t>
         </is>
@@ -1837,9 +1837,9 @@
       <c r="C71" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*B)[i - 2];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 1]) + (*B)[i - 1]) + (*A)[i - 2];
   }
 </t>
         </is>
@@ -1857,9 +1857,9 @@
       <c r="C72" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 2]) + 1 * (*A)[i - 2];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 1]) + (*A)[i - 2];
   }
 </t>
         </is>
@@ -1877,9 +1877,9 @@
       <c r="C73" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*C)[i] = ((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -1897,9 +1897,9 @@
       <c r="C74" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*A)[i - 2]) + 1 * (*B)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2];
+    (*C)[i] = ((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -1917,9 +1917,9 @@
       <c r="C75" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 2];
+    (*B)[i] = (((((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -1937,9 +1937,9 @@
       <c r="C76" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 2]) + 0 * (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = (((((*B)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2]) + (*A)[i - 2];
   }
 </t>
         </is>
@@ -1957,9 +1957,9 @@
       <c r="C77" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1];
+    (*B)[i] = ((((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -1977,9 +1977,9 @@
       <c r="C78" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2]) + (*B)[i - 2]) + (*A)[i - 2];
+    (*B)[i] = (((((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -1997,9 +1997,9 @@
       <c r="C79" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (((((*B)[i - 2] + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2017,9 +2017,9 @@
       <c r="C80" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 3]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 1];
+    (*B)[i] = (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
   }
 </t>
         </is>
@@ -2037,9 +2037,9 @@
       <c r="C81" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*B)[i] = (*B)[i - 3] + (*B)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3];
   }
 </t>
         </is>
@@ -2057,9 +2057,9 @@
       <c r="C82" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*A)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2077,9 +2077,9 @@
       <c r="C83" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*B)[i - 1];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
   }
 </t>
         </is>
@@ -2097,9 +2097,9 @@
       <c r="C84" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = ((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2117,9 +2117,9 @@
       <c r="C85" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 3]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 3];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 3]) + (*C)[i - 2];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*A)[i - 3];
   }
 </t>
         </is>
@@ -2137,9 +2137,9 @@
       <c r="C86" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 2]) + 0 * (*A)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 3] + (*B)[i - 2]) + (*B)[i - 2];
+    (*A)[i] = ((((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -2157,9 +2157,9 @@
       <c r="C87" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*A)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 3]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2177,9 +2177,9 @@
       <c r="C88" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2];
+    (*A)[i] = ((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -2197,9 +2197,9 @@
       <c r="C89" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*A)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 2]) + (*B)[i - 2];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -2217,9 +2217,9 @@
       <c r="C90" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 3];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 3]) + (*B)[i - 1];
+    (*B)[i] = (((((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 3];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 3]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2237,9 +2237,9 @@
       <c r="C91" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 2]) + 1 * (*A)[i - 3]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 3]) + (*B)[i - 1];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 3]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2257,9 +2257,9 @@
       <c r="C92" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 3]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 2]) + 1 * (*B)[i - 3]) + 1 * (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 3]) + (*B)[i - 3]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 3]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 2]) + (*B)[i - 3]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -2277,9 +2277,9 @@
       <c r="C93" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + 0 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3];
+    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 3]) + (*B)[i - 2]) + (*A)[i - 2]) + (*A)[i - 3];
+    (*B)[i] = ((((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2297,9 +2297,9 @@
       <c r="C94" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*A)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 3]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
+    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 3]) + (*B)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*B)[i] = (((((*B)[i - 3] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 3];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2317,9 +2317,9 @@
       <c r="C95" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*C)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2337,9 +2337,9 @@
       <c r="C96" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*C)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2357,9 +2357,9 @@
       <c r="C97" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2377,9 +2377,9 @@
       <c r="C98" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2397,9 +2397,9 @@
       <c r="C99" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 1];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 1];
+    (*B)[i] = (*B)[i - 1] + (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -2417,9 +2417,9 @@
       <c r="C100" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*C)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2437,9 +2437,9 @@
       <c r="C101" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*C)[i] = (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*B)[i] = (((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2457,9 +2457,9 @@
       <c r="C102" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*C)[i] = (((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
+    (*B)[i] = ((*B)[i - 1] + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2477,9 +2477,9 @@
       <c r="C103" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2497,9 +2497,9 @@
       <c r="C104" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*B)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*C)[i] = ((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1]) + (*C)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2517,9 +2517,9 @@
       <c r="C105" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2537,9 +2537,9 @@
       <c r="C106" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1];
+    (*B)[i] = ((((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -2557,9 +2557,9 @@
       <c r="C107" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*B)[i - 1];
+    (*A)[i] = ((((*A)[i - 1] + (*B)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*C)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2577,9 +2577,9 @@
       <c r="C108" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 1] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 1] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 1] + (*B)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (((((*B)[i - 1] + (*C)[i - 1]) + (*B)[i - 1]) + (*B)[i - 1]) + (*C)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2597,9 +2597,9 @@
       <c r="C109" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -2617,9 +2617,9 @@
       <c r="C110" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 2]) + 0 * (*B)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1];
+    (*A)[i] = ((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -2637,9 +2637,9 @@
       <c r="C111" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 1];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
   }
 </t>
         </is>
@@ -2657,9 +2657,9 @@
       <c r="C112" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
+    (*B)[i] = ((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 2];
+    (*A)[i] = ((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1];
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2677,9 +2677,9 @@
       <c r="C113" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*C)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 1];
+    (*B)[i] = ((*B)[i - 2] + (*C)[i - 2]) + (*C)[i - 2];
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -2697,9 +2697,9 @@
       <c r="C114" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*B)[i] = ((*B)[i - 2] + (*C)[i - 2]) + (*C)[i - 2];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -2717,9 +2717,9 @@
       <c r="C115" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = (((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2737,9 +2737,9 @@
       <c r="C116" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1];
+    (*B)[i] = (((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*A)[i - 1];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2757,9 +2757,9 @@
       <c r="C117" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1];
+    (*B)[i] = (((*B)[i - 2] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -2777,9 +2777,9 @@
       <c r="C118" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 2];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 1]) + (*A)[i - 1];
+    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 1]) + (*C)[i - 2]) + (*B)[i - 2]) + (*B)[i - 2];
+    (*C)[i] = (((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -2797,9 +2797,9 @@
       <c r="C119" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 0 * (*B)[i - 2]) + 1 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 1 * (*A)[i - 1];
+    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1]) + (*C)[i - 1]) + (*B)[i - 2];
+    (*C)[i] = ((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1];
   }
 </t>
         </is>
@@ -2817,9 +2817,9 @@
       <c r="C120" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 1];
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*C)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 1]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
+    (*A)[i] = ((((*A)[i - 2] + (*B)[i - 2]) + (*A)[i - 2]) + (*B)[i - 2]) + (*B)[i - 1];
+    (*B)[i] = ((((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 1]) + (*C)[i - 2]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -2837,9 +2837,9 @@
       <c r="C121" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*C)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*B)[i - 1]) + (*C)[i - 2];
+    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1]) + (*A)[i - 1];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -2857,9 +2857,9 @@
       <c r="C122" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 2] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2];
+    (*B)[i] = (((((*B)[i - 2] + (*C)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1]) + (*B)[i - 2];
+    (*A)[i] = (((((*A)[i - 2] + (*B)[i - 2]) + (*B)[i - 2]) + (*A)[i - 2]) + (*A)[i - 1]) + (*B)[i - 2];
+    (*C)[i] = (((((*C)[i - 2] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -2877,9 +2877,9 @@
       <c r="C123" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*B)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2897,9 +2897,9 @@
       <c r="C124" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 2]) + 0 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*C)[i - 1];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2917,9 +2917,9 @@
       <c r="C125" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*A)[i - 3]) + 0 * (*A)[i - 2]) + 0 * (*A)[i - 2]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 3]) + 0 * (*B)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2937,9 +2937,9 @@
       <c r="C126" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 0 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 0 * (*B)[i - 2];
+    (*B)[i] = ((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 3];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
   }
 </t>
         </is>
@@ -2957,9 +2957,9 @@
       <c r="C127" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 1]) + 0 * (*A)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 3]) + 0 * (*C)[i - 3]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*C)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2];
+    (*A)[i] = ((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 1];
+    (*C)[i] = ((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -2977,9 +2977,9 @@
       <c r="C128" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 0 * (*B)[i - 2]) + 0 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*A)[i - 1]) + 0 * (*A)[i - 1]) + 0 * (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 3];
+    (*B)[i] = (((*B)[i - 3] + (*C)[i - 3]) + (*B)[i - 1]) + (*B)[i - 1];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
   }
 </t>
         </is>
@@ -2997,9 +2997,9 @@
       <c r="C129" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 1 * (*A)[i - 1]) + 0 * (*A)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 3]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*C)[i - 1]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 1]) + 1 * (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 1];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 2]) + (*C)[i - 1];
+    (*B)[i] = (((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 2];
   }
 </t>
         </is>
@@ -3017,9 +3017,9 @@
       <c r="C130" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 2]) + 0 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 3]) + 0 * (*B)[i - 2]) + 1 * (*B)[i - 3]) + 1 * (*A)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*B)[i - 1]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 1];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 3]) + (*C)[i - 2];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 3]) + (*A)[i - 3];
+    (*B)[i] = (((*B)[i - 3] + (*C)[i - 3]) + (*B)[i - 1]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -3037,9 +3037,9 @@
       <c r="C131" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 3]) + 0 * (*B)[i - 1];
-    (*C)[i] = (((((*C)[i - 3] + 0 * (*C)[i - 1]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 1]) + 0 * (*A)[i - 3]) + 1 * (*B)[i - 2];
+    (*B)[i] = ((((*B)[i - 3] + (*C)[i - 3]) + (*B)[i - 3]) + (*B)[i - 3]) + (*B)[i - 3];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 1]) + (*C)[i - 1];
+    (*A)[i] = (((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 1]) + (*B)[i - 2];
   }
 </t>
         </is>
@@ -3057,9 +3057,9 @@
       <c r="C132" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 2]) + 0 * (*A)[i - 3]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 3];
+    (*B)[i] = ((((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 1]) + (*B)[i - 3]) + (*B)[i - 2];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 3];
+    (*A)[i] = ((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -3077,9 +3077,9 @@
       <c r="C133" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 0 * (*B)[i - 3]) + 1 * (*A)[i - 2]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 2]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1]) + 0 * (*C)[i - 1]) + 0 * (*C)[i - 3];
+    (*A)[i] = ((((*A)[i - 3] + (*B)[i - 3]) + (*A)[i - 2]) + (*B)[i - 3]) + (*B)[i - 1];
+    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + (*B)[i - 2]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 3];
+    (*C)[i] = (((*C)[i - 3] + (*C)[i - 2]) + (*C)[i - 2]) + (*C)[i - 1];
   }
 </t>
         </is>
@@ -3097,9 +3097,9 @@
       <c r="C134" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 3]) + 0 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*C)[i - 2]) + 1 * (*B)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*B)[i - 2];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 1]) + 1 * (*A)[i - 1]) + 0 * (*B)[i - 3]) + 1 * (*B)[i - 3];
+    (*C)[i] = ((((*C)[i - 3] + (*C)[i - 3]) + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 2];
+    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 2]) + (*B)[i - 1]) + (*B)[i - 3]) + (*B)[i - 2];
+    (*A)[i] = ((((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 1]) + (*A)[i - 1]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -3117,9 +3117,9 @@
       <c r="C135" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 2];
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 1];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*B)[i - 2]) + 1 * (*B)[i - 1]) + 0 * (*C)[i - 2];
+    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*A)[i - 1]) + (*B)[i - 2]) + (*A)[i - 2];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 1];
+    (*B)[i] = ((((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 1]) + (*B)[i - 2]) + (*B)[i - 1];
   }
 </t>
         </is>
@@ -3137,9 +3137,9 @@
       <c r="C136" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (((((*C)[i - 3] + 1 * (*C)[i - 1]) + 1 * (*C)[i - 3]) + 1 * (*C)[i - 1]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3];
-    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + 1 * (*C)[i - 2]) + 1 * (*C)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*C)[i - 1];
-    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + 1 * (*B)[i - 2]) + 1 * (*A)[i - 1]) + 1 * (*B)[i - 3]) + 1 * (*A)[i - 3];
+    (*C)[i] = (((((*C)[i - 3] + (*C)[i - 1]) + (*C)[i - 3]) + (*C)[i - 1]) + (*C)[i - 2]) + (*C)[i - 3];
+    (*B)[i] = (((((*B)[i - 3] + (*C)[i - 3]) + (*C)[i - 2]) + (*C)[i - 3]) + (*B)[i - 2]) + (*C)[i - 1];
+    (*A)[i] = (((((*A)[i - 3] + (*B)[i - 3]) + (*B)[i - 2]) + (*A)[i - 1]) + (*B)[i - 3]) + (*A)[i - 3];
   }
 </t>
         </is>

</xml_diff>